<commit_message>
Merged current master into TC branch
</commit_message>
<xml_diff>
--- a/templates/bulk_import_template.xlsx
+++ b/templates/bulk_import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlynn\Aspace\archivesspace\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDE2258-ACC6-45CD-9E64-1328B7E22440}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C63E88A7-E0C0-415F-949E-F7B7C909027C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="816" windowWidth="18432" windowHeight="11544" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1374" yWindow="1386" windowWidth="19728" windowHeight="10842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="407">
   <si>
     <t>Mapping - ArchivesSpace Resource record SECTION</t>
   </si>
@@ -1241,6 +1241,17 @@
   </si>
   <si>
     <t>res_uri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital Object Identifier
+(Leave this blank to get a default system-assigned Digital Object Identifier that is based on the Archival Object Ref ID. Or enter a custom identifier here to override the default. Custom identifier must be unique within ArchivesSpace.  Note that Digital Object Identifiers are not exported in the EAD.)
+</t>
+  </si>
+  <si>
+    <t>digital_object_id</t>
+  </si>
+  <si>
+    <t>Digital Object ID</t>
   </si>
 </sst>
 </file>
@@ -1543,7 +1554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1755,6 +1766,18 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2177,11 +2200,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQP7"/>
+  <dimension ref="A1:AQQ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AU1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="BJ2" sqref="BJ2:BJ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2230,84 +2253,85 @@
     <col min="59" max="59" width="19.15625" style="50" customWidth="1"/>
     <col min="60" max="60" width="10.41796875" style="1" customWidth="1"/>
     <col min="61" max="61" width="11.41796875" style="50" customWidth="1"/>
-    <col min="62" max="62" width="10.41796875" style="1" customWidth="1"/>
-    <col min="63" max="64" width="9.15625" style="1"/>
-    <col min="65" max="65" width="15.26171875" style="1" customWidth="1"/>
-    <col min="66" max="66" width="22.68359375" style="1"/>
-    <col min="67" max="67" width="15.26171875" style="1" customWidth="1"/>
-    <col min="68" max="68" width="13" style="1" customWidth="1"/>
-    <col min="69" max="69" width="15.41796875" style="1" customWidth="1"/>
-    <col min="70" max="70" width="22.68359375" style="1"/>
-    <col min="71" max="71" width="15.26171875" style="1" customWidth="1"/>
-    <col min="72" max="72" width="9.15625" style="1"/>
-    <col min="73" max="73" width="15.15625" style="1" customWidth="1"/>
-    <col min="74" max="74" width="20.15625" style="1" customWidth="1"/>
-    <col min="75" max="75" width="15.26171875" style="1" customWidth="1"/>
-    <col min="76" max="76" width="12.83984375" style="1" customWidth="1"/>
-    <col min="77" max="77" width="15.15625" style="1" customWidth="1"/>
-    <col min="78" max="78" width="20.15625" style="1" customWidth="1"/>
-    <col min="79" max="79" width="15.26171875" style="1" customWidth="1"/>
-    <col min="80" max="80" width="12.83984375" style="1" customWidth="1"/>
-    <col min="81" max="81" width="15.15625" style="1" customWidth="1"/>
-    <col min="82" max="82" width="20.15625" style="1" customWidth="1"/>
-    <col min="83" max="83" width="15.26171875" style="1" customWidth="1"/>
-    <col min="84" max="84" width="12.83984375" style="1" customWidth="1"/>
-    <col min="85" max="85" width="9.15625" style="1"/>
-    <col min="86" max="86" width="11.41796875" style="1" customWidth="1"/>
-    <col min="87" max="87" width="15.26171875" style="1" customWidth="1"/>
-    <col min="88" max="89" width="9.15625" style="1"/>
-    <col min="90" max="90" width="11.41796875" style="1" customWidth="1"/>
-    <col min="91" max="91" width="15.26171875" style="1" customWidth="1"/>
-    <col min="92" max="94" width="9.15625" style="1"/>
-    <col min="95" max="95" width="15.26171875" style="1" customWidth="1"/>
-    <col min="96" max="98" width="9.15625" style="1"/>
-    <col min="99" max="99" width="15.26171875" style="1" customWidth="1"/>
-    <col min="100" max="102" width="9.15625" style="1"/>
-    <col min="103" max="103" width="15.26171875" style="1" customWidth="1"/>
-    <col min="104" max="104" width="9.15625" style="1"/>
-    <col min="105" max="105" width="11.578125" style="1" customWidth="1"/>
-    <col min="106" max="106" width="12.26171875" style="1" customWidth="1"/>
-    <col min="107" max="109" width="13.578125" style="1" customWidth="1"/>
-    <col min="110" max="111" width="10.83984375" style="1" customWidth="1"/>
-    <col min="112" max="112" width="15.41796875" style="1" customWidth="1"/>
-    <col min="113" max="113" width="9.26171875" style="1"/>
-    <col min="114" max="114" width="17.68359375" style="1" customWidth="1"/>
-    <col min="115" max="115" width="17" style="1" customWidth="1"/>
-    <col min="116" max="116" width="17.68359375" style="1" customWidth="1"/>
-    <col min="117" max="117" width="12.26171875" style="1" customWidth="1"/>
-    <col min="118" max="118" width="17.68359375" style="1" customWidth="1"/>
-    <col min="119" max="119" width="11.68359375" style="1" customWidth="1"/>
-    <col min="120" max="120" width="17.68359375" style="1" customWidth="1"/>
-    <col min="121" max="121" width="16" style="1" customWidth="1"/>
-    <col min="122" max="122" width="17.68359375" style="1" customWidth="1"/>
-    <col min="123" max="123" width="9.15625" style="1"/>
-    <col min="124" max="124" width="17.68359375" style="1" customWidth="1"/>
-    <col min="125" max="125" width="12" customWidth="1"/>
-    <col min="126" max="126" width="17.68359375" style="1" customWidth="1"/>
-    <col min="127" max="127" width="11.83984375" style="1" customWidth="1"/>
-    <col min="128" max="128" width="17.68359375" style="1" customWidth="1"/>
-    <col min="129" max="129" width="11.83984375" style="1" customWidth="1"/>
-    <col min="130" max="130" width="17.68359375" style="1" customWidth="1"/>
-    <col min="131" max="131" width="11.83984375" style="1" customWidth="1"/>
-    <col min="132" max="132" width="17.68359375" style="1" customWidth="1"/>
-    <col min="133" max="133" width="11.83984375" style="1" customWidth="1"/>
-    <col min="134" max="134" width="17.68359375" style="1" customWidth="1"/>
-    <col min="135" max="135" width="14.83984375" style="1" customWidth="1"/>
-    <col min="136" max="136" width="17.68359375" style="1" customWidth="1"/>
-    <col min="137" max="137" width="12.26171875" style="1" customWidth="1"/>
-    <col min="138" max="138" width="17.68359375" style="1" customWidth="1"/>
-    <col min="139" max="139" width="9.15625" style="1"/>
-    <col min="140" max="140" width="17.68359375" style="1" customWidth="1"/>
-    <col min="141" max="141" width="9.15625" style="1"/>
-    <col min="142" max="142" width="17.68359375" style="1" customWidth="1"/>
-    <col min="143" max="143" width="18.41796875" style="1" customWidth="1"/>
-    <col min="144" max="144" width="17.68359375" style="1" customWidth="1"/>
-    <col min="145" max="145" width="10.15625" style="1" customWidth="1"/>
-    <col min="146" max="146" width="17.68359375" style="1" customWidth="1"/>
-    <col min="147" max="1134" width="9.26171875" style="1"/>
+    <col min="62" max="62" width="15.83984375" style="63" customWidth="1"/>
+    <col min="63" max="63" width="10.41796875" style="1" customWidth="1"/>
+    <col min="64" max="65" width="9.15625" style="1"/>
+    <col min="66" max="66" width="15.26171875" style="1" customWidth="1"/>
+    <col min="67" max="67" width="22.68359375" style="1"/>
+    <col min="68" max="68" width="15.26171875" style="1" customWidth="1"/>
+    <col min="69" max="69" width="13" style="1" customWidth="1"/>
+    <col min="70" max="70" width="15.41796875" style="1" customWidth="1"/>
+    <col min="71" max="71" width="22.68359375" style="1"/>
+    <col min="72" max="72" width="15.26171875" style="1" customWidth="1"/>
+    <col min="73" max="73" width="9.15625" style="1"/>
+    <col min="74" max="74" width="15.15625" style="1" customWidth="1"/>
+    <col min="75" max="75" width="20.15625" style="1" customWidth="1"/>
+    <col min="76" max="76" width="15.26171875" style="1" customWidth="1"/>
+    <col min="77" max="77" width="12.83984375" style="1" customWidth="1"/>
+    <col min="78" max="78" width="15.15625" style="1" customWidth="1"/>
+    <col min="79" max="79" width="20.15625" style="1" customWidth="1"/>
+    <col min="80" max="80" width="15.26171875" style="1" customWidth="1"/>
+    <col min="81" max="81" width="12.83984375" style="1" customWidth="1"/>
+    <col min="82" max="82" width="15.15625" style="1" customWidth="1"/>
+    <col min="83" max="83" width="20.15625" style="1" customWidth="1"/>
+    <col min="84" max="84" width="15.26171875" style="1" customWidth="1"/>
+    <col min="85" max="85" width="12.83984375" style="1" customWidth="1"/>
+    <col min="86" max="86" width="9.15625" style="1"/>
+    <col min="87" max="87" width="11.41796875" style="1" customWidth="1"/>
+    <col min="88" max="88" width="15.26171875" style="1" customWidth="1"/>
+    <col min="89" max="90" width="9.15625" style="1"/>
+    <col min="91" max="91" width="11.41796875" style="1" customWidth="1"/>
+    <col min="92" max="92" width="15.26171875" style="1" customWidth="1"/>
+    <col min="93" max="95" width="9.15625" style="1"/>
+    <col min="96" max="96" width="15.26171875" style="1" customWidth="1"/>
+    <col min="97" max="99" width="9.15625" style="1"/>
+    <col min="100" max="100" width="15.26171875" style="1" customWidth="1"/>
+    <col min="101" max="103" width="9.15625" style="1"/>
+    <col min="104" max="104" width="15.26171875" style="1" customWidth="1"/>
+    <col min="105" max="105" width="9.15625" style="1"/>
+    <col min="106" max="106" width="11.578125" style="1" customWidth="1"/>
+    <col min="107" max="107" width="12.26171875" style="1" customWidth="1"/>
+    <col min="108" max="110" width="13.578125" style="1" customWidth="1"/>
+    <col min="111" max="112" width="10.83984375" style="1" customWidth="1"/>
+    <col min="113" max="113" width="15.41796875" style="1" customWidth="1"/>
+    <col min="114" max="114" width="9.26171875" style="1"/>
+    <col min="115" max="115" width="17.68359375" style="1" customWidth="1"/>
+    <col min="116" max="116" width="17" style="1" customWidth="1"/>
+    <col min="117" max="117" width="17.68359375" style="1" customWidth="1"/>
+    <col min="118" max="118" width="12.26171875" style="1" customWidth="1"/>
+    <col min="119" max="119" width="17.68359375" style="1" customWidth="1"/>
+    <col min="120" max="120" width="11.68359375" style="1" customWidth="1"/>
+    <col min="121" max="121" width="17.68359375" style="1" customWidth="1"/>
+    <col min="122" max="122" width="16" style="1" customWidth="1"/>
+    <col min="123" max="123" width="17.68359375" style="1" customWidth="1"/>
+    <col min="124" max="124" width="9.15625" style="1"/>
+    <col min="125" max="125" width="17.68359375" style="1" customWidth="1"/>
+    <col min="126" max="126" width="12" customWidth="1"/>
+    <col min="127" max="127" width="17.68359375" style="1" customWidth="1"/>
+    <col min="128" max="128" width="11.83984375" style="1" customWidth="1"/>
+    <col min="129" max="129" width="17.68359375" style="1" customWidth="1"/>
+    <col min="130" max="130" width="11.83984375" style="1" customWidth="1"/>
+    <col min="131" max="131" width="17.68359375" style="1" customWidth="1"/>
+    <col min="132" max="132" width="11.83984375" style="1" customWidth="1"/>
+    <col min="133" max="133" width="17.68359375" style="1" customWidth="1"/>
+    <col min="134" max="134" width="11.83984375" style="1" customWidth="1"/>
+    <col min="135" max="135" width="17.68359375" style="1" customWidth="1"/>
+    <col min="136" max="136" width="14.83984375" style="1" customWidth="1"/>
+    <col min="137" max="137" width="17.68359375" style="1" customWidth="1"/>
+    <col min="138" max="138" width="12.26171875" style="1" customWidth="1"/>
+    <col min="139" max="139" width="17.68359375" style="1" customWidth="1"/>
+    <col min="140" max="140" width="9.15625" style="1"/>
+    <col min="141" max="141" width="17.68359375" style="1" customWidth="1"/>
+    <col min="142" max="142" width="9.15625" style="1"/>
+    <col min="143" max="143" width="17.68359375" style="1" customWidth="1"/>
+    <col min="144" max="144" width="18.41796875" style="1" customWidth="1"/>
+    <col min="145" max="145" width="17.68359375" style="1" customWidth="1"/>
+    <col min="146" max="146" width="10.15625" style="1" customWidth="1"/>
+    <col min="147" max="147" width="17.68359375" style="1" customWidth="1"/>
+    <col min="148" max="1135" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:146" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:147" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="31" t="s">
         <v>397</v>
       </c>
@@ -2318,7 +2342,7 @@
       <c r="S1" s="64"/>
       <c r="T1" s="64"/>
     </row>
-    <row r="2" spans="1:146" s="1" customFormat="1" ht="51.9" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:147" s="1" customFormat="1" ht="51.9" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
@@ -2502,25 +2526,25 @@
       <c r="BI2" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="BJ2" s="22" t="s">
+      <c r="BJ2" s="72" t="s">
         <v>41</v>
       </c>
       <c r="BK2" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="BL2" s="23" t="s">
+      <c r="BL2" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="BM2" s="48" t="s">
+      <c r="BM2" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="BN2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="BN2" s="19" t="s">
+      <c r="BO2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BO2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="BP2" s="19" t="s">
+      <c r="BP2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BQ2" s="19" t="s">
@@ -2529,10 +2553,10 @@
       <c r="BR2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BS2" s="48" t="s">
+      <c r="BS2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BT2" s="19" t="s">
+      <c r="BT2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BU2" s="19" t="s">
@@ -2541,10 +2565,10 @@
       <c r="BV2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BW2" s="48" t="s">
+      <c r="BW2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BX2" s="19" t="s">
+      <c r="BX2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BY2" s="19" t="s">
@@ -2553,10 +2577,10 @@
       <c r="BZ2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CA2" s="48" t="s">
+      <c r="CA2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CB2" s="19" t="s">
+      <c r="CB2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="CC2" s="19" t="s">
@@ -2565,10 +2589,10 @@
       <c r="CD2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CE2" s="48" t="s">
+      <c r="CE2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CF2" s="19" t="s">
+      <c r="CF2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="CG2" s="19" t="s">
@@ -2577,10 +2601,10 @@
       <c r="CH2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CI2" s="48" t="s">
+      <c r="CI2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CJ2" s="19" t="s">
+      <c r="CJ2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="CK2" s="19" t="s">
@@ -2589,10 +2613,10 @@
       <c r="CL2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CM2" s="48" t="s">
+      <c r="CM2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CN2" s="19" t="s">
+      <c r="CN2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="CO2" s="19" t="s">
@@ -2601,10 +2625,10 @@
       <c r="CP2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CQ2" s="48" t="s">
+      <c r="CQ2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CR2" s="19" t="s">
+      <c r="CR2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="CS2" s="19" t="s">
@@ -2613,10 +2637,10 @@
       <c r="CT2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CU2" s="48" t="s">
+      <c r="CU2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CV2" s="19" t="s">
+      <c r="CV2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="CW2" s="19" t="s">
@@ -2625,14 +2649,14 @@
       <c r="CX2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CY2" s="48" t="s">
+      <c r="CY2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CZ2" s="19" t="s">
+      <c r="CZ2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="DA2" s="21" t="s">
-        <v>120</v>
+      <c r="DA2" s="19" t="s">
+        <v>1</v>
       </c>
       <c r="DB2" s="21" t="s">
         <v>120</v>
@@ -2655,8 +2679,8 @@
       <c r="DH2" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="DI2" s="29" t="s">
-        <v>65</v>
+      <c r="DI2" s="21" t="s">
+        <v>120</v>
       </c>
       <c r="DJ2" s="29" t="s">
         <v>65</v>
@@ -2679,10 +2703,10 @@
       <c r="DP2" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="DQ2" s="28" t="s">
+      <c r="DQ2" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="DR2" s="29" t="s">
+      <c r="DR2" s="28" t="s">
         <v>65</v>
       </c>
       <c r="DS2" s="29" t="s">
@@ -2721,10 +2745,10 @@
       <c r="ED2" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="EE2" s="30" t="s">
+      <c r="EE2" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="EF2" s="29" t="s">
+      <c r="EF2" s="30" t="s">
         <v>65</v>
       </c>
       <c r="EG2" s="29" t="s">
@@ -2757,8 +2781,11 @@
       <c r="EP2" s="29" t="s">
         <v>65</v>
       </c>
+      <c r="EQ2" s="29" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="3" spans="1:146" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:147" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="34" t="s">
         <v>68</v>
       </c>
@@ -2940,263 +2967,266 @@
       <c r="BI3" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="BJ3" s="24" t="s">
+      <c r="BJ3" s="73" t="s">
+        <v>404</v>
+      </c>
+      <c r="BK3" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="BK3" s="25" t="s">
+      <c r="BL3" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="BL3" s="24" t="s">
+      <c r="BM3" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="BM3" s="27" t="s">
+      <c r="BN3" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="BN3" s="27" t="s">
+      <c r="BO3" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="BO3" s="27" t="s">
+      <c r="BP3" s="27" t="s">
         <v>259</v>
       </c>
-      <c r="BP3" s="27" t="s">
+      <c r="BQ3" s="27" t="s">
         <v>287</v>
       </c>
-      <c r="BQ3" s="27" t="s">
+      <c r="BR3" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="BR3" s="27" t="s">
+      <c r="BS3" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="BS3" s="27" t="s">
+      <c r="BT3" s="27" t="s">
         <v>259</v>
       </c>
-      <c r="BT3" s="27" t="s">
+      <c r="BU3" s="27" t="s">
         <v>288</v>
       </c>
-      <c r="BU3" s="27" t="s">
+      <c r="BV3" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="BV3" s="27" t="s">
+      <c r="BW3" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="BW3" s="27" t="s">
+      <c r="BX3" s="27" t="s">
         <v>259</v>
       </c>
-      <c r="BX3" s="27" t="s">
+      <c r="BY3" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="BY3" s="27" t="s">
+      <c r="BZ3" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="BZ3" s="27" t="s">
+      <c r="CA3" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="CA3" s="27" t="s">
+      <c r="CB3" s="27" t="s">
         <v>259</v>
       </c>
-      <c r="CB3" s="27" t="s">
+      <c r="CC3" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="CC3" s="27" t="s">
+      <c r="CD3" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="CD3" s="27" t="s">
+      <c r="CE3" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="CE3" s="27" t="s">
+      <c r="CF3" s="27" t="s">
         <v>259</v>
       </c>
-      <c r="CF3" s="27" t="s">
+      <c r="CG3" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="CG3" s="27" t="s">
+      <c r="CH3" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="CH3" s="27" t="s">
+      <c r="CI3" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="CI3" s="27" t="s">
+      <c r="CJ3" s="27" t="s">
         <v>279</v>
       </c>
-      <c r="CJ3" s="27" t="s">
+      <c r="CK3" s="27" t="s">
         <v>281</v>
       </c>
-      <c r="CK3" s="27" t="s">
+      <c r="CL3" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="CL3" s="27" t="s">
+      <c r="CM3" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="CM3" s="27" t="s">
+      <c r="CN3" s="27" t="s">
         <v>279</v>
       </c>
-      <c r="CN3" s="27" t="s">
+      <c r="CO3" s="27" t="s">
         <v>281</v>
       </c>
-      <c r="CO3" s="27" t="s">
+      <c r="CP3" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="CP3" s="27" t="s">
+      <c r="CQ3" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="CQ3" s="27" t="s">
+      <c r="CR3" s="27" t="s">
         <v>283</v>
       </c>
-      <c r="CR3" s="27" t="s">
+      <c r="CS3" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="CS3" s="27" t="s">
+      <c r="CT3" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="CT3" s="27" t="s">
+      <c r="CU3" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="CU3" s="27" t="s">
+      <c r="CV3" s="27" t="s">
         <v>283</v>
       </c>
-      <c r="CV3" s="27" t="s">
+      <c r="CW3" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="CW3" s="27" t="s">
+      <c r="CX3" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="CX3" s="27" t="s">
+      <c r="CY3" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="CY3" s="27" t="s">
+      <c r="CZ3" s="27" t="s">
         <v>283</v>
       </c>
-      <c r="CZ3" s="27" t="s">
+      <c r="DA3" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="DA3" s="62" t="s">
+      <c r="DB3" s="62" t="s">
         <v>163</v>
       </c>
-      <c r="DB3" s="62" t="s">
+      <c r="DC3" s="62" t="s">
         <v>398</v>
       </c>
-      <c r="DC3" s="62" t="s">
+      <c r="DD3" s="62" t="s">
         <v>399</v>
       </c>
-      <c r="DD3" s="62" t="s">
+      <c r="DE3" s="62" t="s">
         <v>179</v>
       </c>
-      <c r="DE3" s="62" t="s">
+      <c r="DF3" s="62" t="s">
         <v>163</v>
       </c>
-      <c r="DF3" s="62" t="s">
+      <c r="DG3" s="62" t="s">
         <v>398</v>
       </c>
-      <c r="DG3" s="62" t="s">
+      <c r="DH3" s="62" t="s">
         <v>399</v>
       </c>
-      <c r="DH3" s="62" t="s">
+      <c r="DI3" s="62" t="s">
         <v>179</v>
       </c>
-      <c r="DI3" s="26" t="s">
+      <c r="DJ3" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="DJ3" s="59" t="s">
+      <c r="DK3" s="59" t="s">
         <v>239</v>
       </c>
-      <c r="DK3" s="26" t="s">
+      <c r="DL3" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="DL3" s="59" t="s">
+      <c r="DM3" s="59" t="s">
         <v>237</v>
       </c>
-      <c r="DM3" s="26" t="s">
+      <c r="DN3" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="DN3" s="59" t="s">
+      <c r="DO3" s="59" t="s">
         <v>235</v>
       </c>
-      <c r="DO3" s="26" t="s">
+      <c r="DP3" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="DP3" s="59" t="s">
+      <c r="DQ3" s="59" t="s">
         <v>233</v>
       </c>
-      <c r="DQ3" s="26" t="s">
+      <c r="DR3" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="DR3" s="59" t="s">
+      <c r="DS3" s="59" t="s">
         <v>231</v>
       </c>
-      <c r="DS3" s="26" t="s">
+      <c r="DT3" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="DT3" s="59" t="s">
+      <c r="DU3" s="59" t="s">
         <v>229</v>
       </c>
-      <c r="DU3" s="26" t="s">
+      <c r="DV3" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="DV3" s="59" t="s">
+      <c r="DW3" s="59" t="s">
         <v>227</v>
       </c>
-      <c r="DW3" s="26" t="s">
+      <c r="DX3" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="DX3" s="59" t="s">
+      <c r="DY3" s="59" t="s">
         <v>225</v>
       </c>
-      <c r="DY3" s="26" t="s">
+      <c r="DZ3" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="DZ3" s="59" t="s">
+      <c r="EA3" s="59" t="s">
         <v>223</v>
       </c>
-      <c r="EA3" s="26" t="s">
+      <c r="EB3" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="EB3" s="59" t="s">
+      <c r="EC3" s="59" t="s">
         <v>221</v>
       </c>
-      <c r="EC3" s="26" t="s">
+      <c r="ED3" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="ED3" s="59" t="s">
+      <c r="EE3" s="59" t="s">
         <v>219</v>
       </c>
-      <c r="EE3" s="26" t="s">
+      <c r="EF3" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="EF3" s="59" t="s">
+      <c r="EG3" s="59" t="s">
         <v>217</v>
       </c>
-      <c r="EG3" s="26" t="s">
+      <c r="EH3" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="EH3" s="59" t="s">
+      <c r="EI3" s="59" t="s">
         <v>216</v>
       </c>
-      <c r="EI3" s="26" t="s">
+      <c r="EJ3" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="EJ3" s="59" t="s">
+      <c r="EK3" s="59" t="s">
         <v>212</v>
       </c>
-      <c r="EK3" s="26" t="s">
+      <c r="EL3" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="EL3" s="59" t="s">
+      <c r="EM3" s="59" t="s">
         <v>211</v>
       </c>
-      <c r="EM3" s="26" t="s">
+      <c r="EN3" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="EN3" s="59" t="s">
+      <c r="EO3" s="59" t="s">
         <v>209</v>
       </c>
-      <c r="EO3" s="26" t="s">
+      <c r="EP3" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="EP3" s="59" t="s">
+      <c r="EQ3" s="59" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:146" s="60" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:147" s="60" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="36" t="s">
         <v>5</v>
       </c>
@@ -3380,263 +3410,266 @@
       <c r="BI4" s="40" t="s">
         <v>375</v>
       </c>
-      <c r="BJ4" s="38" t="s">
+      <c r="BJ4" s="74" t="s">
+        <v>405</v>
+      </c>
+      <c r="BK4" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="BK4" s="38" t="s">
+      <c r="BL4" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="BL4" s="38" t="s">
+      <c r="BM4" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="BM4" s="38" t="s">
+      <c r="BN4" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="BN4" s="38" t="s">
+      <c r="BO4" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="BO4" s="38" t="s">
+      <c r="BP4" s="38" t="s">
         <v>260</v>
       </c>
-      <c r="BP4" s="38" t="s">
+      <c r="BQ4" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="BQ4" s="38" t="s">
+      <c r="BR4" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="BR4" s="38" t="s">
+      <c r="BS4" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="BS4" s="38" t="s">
+      <c r="BT4" s="38" t="s">
         <v>274</v>
       </c>
-      <c r="BT4" s="38" t="s">
+      <c r="BU4" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="BU4" s="38" t="s">
+      <c r="BV4" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="BV4" s="38" t="s">
+      <c r="BW4" s="38" t="s">
         <v>186</v>
       </c>
-      <c r="BW4" s="38" t="s">
+      <c r="BX4" s="38" t="s">
         <v>277</v>
       </c>
-      <c r="BX4" s="38" t="s">
+      <c r="BY4" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="BY4" s="38" t="s">
+      <c r="BZ4" s="38" t="s">
         <v>313</v>
       </c>
-      <c r="BZ4" s="38" t="s">
+      <c r="CA4" s="38" t="s">
         <v>315</v>
       </c>
-      <c r="CA4" s="38" t="s">
+      <c r="CB4" s="38" t="s">
         <v>317</v>
       </c>
-      <c r="CB4" s="38" t="s">
+      <c r="CC4" s="38" t="s">
         <v>319</v>
       </c>
-      <c r="CC4" s="38" t="s">
+      <c r="CD4" s="38" t="s">
         <v>321</v>
       </c>
-      <c r="CD4" s="38" t="s">
+      <c r="CE4" s="38" t="s">
         <v>323</v>
       </c>
-      <c r="CE4" s="38" t="s">
+      <c r="CF4" s="38" t="s">
         <v>325</v>
       </c>
-      <c r="CF4" s="38" t="s">
+      <c r="CG4" s="38" t="s">
         <v>327</v>
       </c>
-      <c r="CG4" s="38" t="s">
+      <c r="CH4" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="CH4" s="38" t="s">
+      <c r="CI4" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="CI4" s="38" t="s">
+      <c r="CJ4" s="38" t="s">
         <v>280</v>
       </c>
-      <c r="CJ4" s="38" t="s">
+      <c r="CK4" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="CK4" s="38" t="s">
+      <c r="CL4" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="CL4" s="38" t="s">
+      <c r="CM4" s="38" t="s">
         <v>296</v>
       </c>
-      <c r="CM4" s="38" t="s">
+      <c r="CN4" s="38" t="s">
         <v>298</v>
       </c>
-      <c r="CN4" s="38" t="s">
+      <c r="CO4" s="38" t="s">
         <v>300</v>
       </c>
-      <c r="CO4" s="38" t="s">
+      <c r="CP4" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="CP4" s="38" t="s">
+      <c r="CQ4" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="CQ4" s="38" t="s">
+      <c r="CR4" s="38" t="s">
         <v>284</v>
       </c>
-      <c r="CR4" s="38" t="s">
+      <c r="CS4" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="CS4" s="38" t="s">
+      <c r="CT4" s="38" t="s">
         <v>191</v>
       </c>
-      <c r="CT4" s="38" t="s">
+      <c r="CU4" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="CU4" s="38" t="s">
+      <c r="CV4" s="38" t="s">
         <v>285</v>
       </c>
-      <c r="CV4" s="38" t="s">
+      <c r="CW4" s="38" t="s">
         <v>192</v>
       </c>
-      <c r="CW4" s="38" t="s">
+      <c r="CX4" s="38" t="s">
         <v>304</v>
       </c>
-      <c r="CX4" s="38" t="s">
+      <c r="CY4" s="38" t="s">
         <v>306</v>
       </c>
-      <c r="CY4" s="38" t="s">
+      <c r="CZ4" s="38" t="s">
         <v>308</v>
       </c>
-      <c r="CZ4" s="38" t="s">
+      <c r="DA4" s="38" t="s">
         <v>310</v>
       </c>
-      <c r="DA4" s="38" t="s">
+      <c r="DB4" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="DB4" s="38" t="s">
+      <c r="DC4" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="DC4" s="38" t="s">
+      <c r="DD4" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="DD4" s="38" t="s">
+      <c r="DE4" s="38" t="s">
         <v>166</v>
       </c>
-      <c r="DE4" s="38" t="s">
+      <c r="DF4" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="DF4" s="38" t="s">
+      <c r="DG4" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="DG4" s="38" t="s">
+      <c r="DH4" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="DH4" s="38" t="s">
+      <c r="DI4" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="DI4" s="38" t="s">
+      <c r="DJ4" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="DJ4" s="38" t="s">
+      <c r="DK4" s="38" t="s">
         <v>241</v>
       </c>
-      <c r="DK4" s="38" t="s">
+      <c r="DL4" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="DL4" s="38" t="s">
+      <c r="DM4" s="38" t="s">
         <v>242</v>
       </c>
-      <c r="DM4" s="41" t="s">
+      <c r="DN4" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="DN4" s="38" t="s">
+      <c r="DO4" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="DO4" s="38" t="s">
+      <c r="DP4" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="DP4" s="38" t="s">
+      <c r="DQ4" s="38" t="s">
         <v>244</v>
       </c>
-      <c r="DQ4" s="38" t="s">
+      <c r="DR4" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="DR4" s="38" t="s">
+      <c r="DS4" s="38" t="s">
         <v>245</v>
       </c>
-      <c r="DS4" s="41" t="s">
+      <c r="DT4" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="DT4" s="38" t="s">
+      <c r="DU4" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="DU4" s="41" t="s">
+      <c r="DV4" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="DV4" s="38" t="s">
+      <c r="DW4" s="38" t="s">
         <v>247</v>
       </c>
-      <c r="DW4" s="41" t="s">
+      <c r="DX4" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="DX4" s="38" t="s">
+      <c r="DY4" s="38" t="s">
         <v>248</v>
       </c>
-      <c r="DY4" s="38" t="s">
+      <c r="DZ4" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="DZ4" s="38" t="s">
+      <c r="EA4" s="38" t="s">
         <v>250</v>
       </c>
-      <c r="EA4" s="38" t="s">
+      <c r="EB4" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="EB4" s="38" t="s">
+      <c r="EC4" s="38" t="s">
         <v>251</v>
       </c>
-      <c r="EC4" s="38" t="s">
+      <c r="ED4" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="ED4" s="38" t="s">
+      <c r="EE4" s="38" t="s">
         <v>252</v>
       </c>
-      <c r="EE4" s="41" t="s">
+      <c r="EF4" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="EF4" s="38" t="s">
+      <c r="EG4" s="38" t="s">
         <v>253</v>
       </c>
-      <c r="EG4" s="38" t="s">
+      <c r="EH4" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="EH4" s="38" t="s">
+      <c r="EI4" s="38" t="s">
         <v>254</v>
       </c>
-      <c r="EI4" s="41" t="s">
+      <c r="EJ4" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="EJ4" s="38" t="s">
+      <c r="EK4" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="EK4" s="38" t="s">
+      <c r="EL4" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="EL4" s="38" t="s">
+      <c r="EM4" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="EM4" s="41" t="s">
+      <c r="EN4" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="EN4" s="41" t="s">
+      <c r="EO4" s="41" t="s">
         <v>257</v>
       </c>
-      <c r="EO4" s="41" t="s">
+      <c r="EP4" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="EP4" s="38" t="s">
+      <c r="EQ4" s="38" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="5" spans="1:146" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:147" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A5" s="35" t="s">
         <v>67</v>
       </c>
@@ -3820,263 +3853,266 @@
       <c r="BI5" s="53" t="s">
         <v>376</v>
       </c>
-      <c r="BJ5" s="4" t="s">
+      <c r="BJ5" s="75" t="s">
+        <v>406</v>
+      </c>
+      <c r="BK5" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="BK5" s="4" t="s">
+      <c r="BL5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="BL5" s="4" t="s">
+      <c r="BM5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="BM5" s="4" t="s">
+      <c r="BN5" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="BN5" s="4" t="s">
+      <c r="BO5" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="BO5" s="4" t="s">
+      <c r="BP5" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="BP5" s="4" t="s">
+      <c r="BQ5" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="BQ5" s="4" t="s">
+      <c r="BR5" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="BR5" s="4" t="s">
+      <c r="BS5" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="BS5" s="4" t="s">
+      <c r="BT5" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="BT5" s="4" t="s">
+      <c r="BU5" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="BU5" s="4" t="s">
+      <c r="BV5" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="BV5" s="4" t="s">
+      <c r="BW5" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="BW5" s="4" t="s">
+      <c r="BX5" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="BX5" s="4" t="s">
+      <c r="BY5" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="BY5" s="4" t="s">
+      <c r="BZ5" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="BZ5" s="4" t="s">
+      <c r="CA5" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="CA5" s="4" t="s">
+      <c r="CB5" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="CB5" s="4" t="s">
+      <c r="CC5" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="CC5" s="4" t="s">
+      <c r="CD5" s="4" t="s">
         <v>322</v>
       </c>
-      <c r="CD5" s="4" t="s">
+      <c r="CE5" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="CE5" s="4" t="s">
+      <c r="CF5" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="CF5" s="4" t="s">
+      <c r="CG5" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="CG5" s="4" t="s">
+      <c r="CH5" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="CH5" s="4" t="s">
+      <c r="CI5" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="CI5" s="4" t="s">
+      <c r="CJ5" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="CJ5" s="4" t="s">
+      <c r="CK5" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="CK5" s="4" t="s">
+      <c r="CL5" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="CL5" s="4" t="s">
+      <c r="CM5" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="CM5" s="4" t="s">
+      <c r="CN5" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="CN5" s="4" t="s">
+      <c r="CO5" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="CO5" s="4" t="s">
+      <c r="CP5" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="CP5" s="4" t="s">
+      <c r="CQ5" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="CQ5" s="4" t="s">
+      <c r="CR5" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="CR5" s="4" t="s">
+      <c r="CS5" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="CS5" s="4" t="s">
+      <c r="CT5" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="CT5" s="4" t="s">
+      <c r="CU5" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="CU5" s="4" t="s">
+      <c r="CV5" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="CV5" s="4" t="s">
+      <c r="CW5" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="CW5" s="4" t="s">
+      <c r="CX5" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="CX5" s="4" t="s">
+      <c r="CY5" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="CY5" s="4" t="s">
+      <c r="CZ5" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="CZ5" s="4" t="s">
+      <c r="DA5" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="DA5" s="4" t="s">
+      <c r="DB5" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="DB5" s="4" t="s">
+      <c r="DC5" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="DC5" s="4" t="s">
+      <c r="DD5" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="DD5" s="4" t="s">
+      <c r="DE5" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="DE5" s="4" t="s">
+      <c r="DF5" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="DF5" s="4" t="s">
+      <c r="DG5" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="DG5" s="4" t="s">
+      <c r="DH5" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="DH5" s="4" t="s">
+      <c r="DI5" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="DI5" s="4" t="s">
+      <c r="DJ5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="DJ5" s="4" t="s">
+      <c r="DK5" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="DK5" s="4" t="s">
+      <c r="DL5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="DL5" s="4" t="s">
+      <c r="DM5" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="DM5" s="7" t="s">
+      <c r="DN5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="DN5" s="4" t="s">
+      <c r="DO5" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="DO5" s="4" t="s">
+      <c r="DP5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="DP5" s="4" t="s">
+      <c r="DQ5" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="DQ5" s="4" t="s">
+      <c r="DR5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="DR5" s="4" t="s">
+      <c r="DS5" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="DS5" s="7" t="s">
+      <c r="DT5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="DT5" s="4" t="s">
+      <c r="DU5" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="DU5" s="7" t="s">
+      <c r="DV5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="DV5" s="4" t="s">
+      <c r="DW5" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="DW5" s="7" t="s">
+      <c r="DX5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="DX5" s="4" t="s">
+      <c r="DY5" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="DY5" s="4" t="s">
+      <c r="DZ5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="DZ5" s="4" t="s">
+      <c r="EA5" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="EA5" s="4" t="s">
+      <c r="EB5" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="EB5" s="4" t="s">
+      <c r="EC5" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="EC5" s="4" t="s">
+      <c r="ED5" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="ED5" s="4" t="s">
+      <c r="EE5" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="EE5" s="14" t="s">
+      <c r="EF5" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="EF5" s="4" t="s">
+      <c r="EG5" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="EG5" s="4" t="s">
+      <c r="EH5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="EH5" s="4" t="s">
+      <c r="EI5" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="EI5" s="7" t="s">
+      <c r="EJ5" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="EJ5" s="4" t="s">
+      <c r="EK5" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="EK5" s="4" t="s">
+      <c r="EL5" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="EL5" s="4" t="s">
+      <c r="EM5" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="EM5" s="7" t="s">
+      <c r="EN5" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="EN5" s="4" t="s">
+      <c r="EO5" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="EO5" s="7" t="s">
+      <c r="EP5" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="EP5" s="4" t="s">
+      <c r="EQ5" s="4" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:146" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:147" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="N6" s="64"/>
       <c r="O6" s="64"/>
       <c r="P6" s="64"/>
@@ -4084,7 +4120,7 @@
       <c r="S6" s="64"/>
       <c r="T6" s="64"/>
     </row>
-    <row r="7" spans="1:146" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:147" x14ac:dyDescent="0.55000000000000004">
       <c r="H7" s="32"/>
       <c r="N7" s="64"/>
       <c r="O7" s="64"/>
@@ -4108,7 +4144,7 @@
       <formula1>1</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="K6:K1048576 EN6:EN1048576 EL6:EL1048576 EP6:EP1048576 EJ6:EJ1048576 EH6:EH1048576 EF6:EF1048576 ED6:ED1048576 EB6:EB1048576 DZ6:DZ1048576 DX6:DX1048576 DV6:DV1048576 DT6:DT1048576 DR6:DR1048576 DP6:DP1048576 DN6:DN1048576 DL6:DL1048576 DJ6:DJ1048576 Q6:Q1048576 U6:U1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="K6:K1048576 EO6:EO1048576 EM6:EM1048576 EQ6:EQ1048576 EK6:EK1048576 EI6:EI1048576 EG6:EG1048576 EE6:EE1048576 EC6:EC1048576 EA6:EA1048576 DY6:DY1048576 DW6:DW1048576 DU6:DU1048576 DS6:DS1048576 DQ6:DQ1048576 DO6:DO1048576 DM6:DM1048576 DK6:DK1048576 Q6:Q1048576 U6:U1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4121,7 +4157,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>BO6:BO1048576 BS6:BS1048576 CI6:CI1048576 BW6:BW1048576 CU6:CU1048576 CM6:CM1048576 CQ6:CQ1048576 CY6:CY1048576 CA6:CA1048576 CE6:CE1048576</xm:sqref>
+          <xm:sqref>BP6:BP1048576 BT6:BT1048576 CJ6:CJ1048576 BX6:BX1048576 CV6:CV1048576 CN6:CN1048576 CR6:CR1048576 CZ6:CZ1048576 CB6:CB1048576 CF6:CF1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Top Container CSV download template Functionality for CSV/XLSX top container uploading for multiple AOs per resource.
Adding in marcxml_converter as an include for main.rb because of missing
marcxml object during testing.

Corrected tests to precreate containers into the container handler hash
to avoid attempts to access via solr.

Removed repo faceting testing because it isn't in this branch.

Merged bulk importing changes from master

Bulk import merge from master

Master bulk import merge

Master merge

Reinstating missing bulk import file

master->branch

Corrected container method

Resolve duplication issues and remove institution specific changes

Set hidden to true and create template for top_container_linker_job

Update jobs toolbar to fix error caused by hidden job

Bulk import job modal refactoring to set job type based on load type
</commit_message>
<xml_diff>
--- a/templates/bulk_import_template.xlsx
+++ b/templates/bulk_import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlynn\Aspace\archivesspace\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDCD5C4-0D63-4C0B-BB62-5A418BF5EB63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250BCDE9-68E9-4741-85B5-9055941E89B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="702" yWindow="714" windowWidth="19728" windowHeight="10842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="407">
   <si>
     <t>Mapping - ArchivesSpace Resource record SECTION</t>
   </si>
@@ -42,6 +42,9 @@
     <t>ArchivesSpace field code (please don't edit this row)</t>
   </si>
   <si>
+    <t>collection_id</t>
+  </si>
+  <si>
     <t>level</t>
   </si>
   <si>
@@ -310,6 +313,12 @@
   </si>
   <si>
     <t>Dates</t>
+  </si>
+  <si>
+    <t>Resource Identifier</t>
+  </si>
+  <si>
+    <t>The Resource "Identifier", aka collection-level unit_id, OR, could be internal resource record number from URL.</t>
   </si>
   <si>
     <t>Archival Object Basic Information</t>
@@ -1249,7 +1258,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1353,12 +1362,19 @@
       <charset val="1"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1393,6 +1409,12 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -1532,7 +1554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1586,7 +1608,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1595,7 +1617,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1604,22 +1626,22 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1637,19 +1659,22 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1660,7 +1685,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1673,7 +1698,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1700,16 +1725,19 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1722,31 +1750,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2172,350 +2200,351 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQP7"/>
+  <dimension ref="A1:AQQ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="AU1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BJ2" sqref="BJ2:BJ5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="31" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="61" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="30.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" style="44" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" style="1" customWidth="1"/>
-    <col min="13" max="15" width="14.28515625" style="61" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" style="61" customWidth="1"/>
-    <col min="17" max="19" width="14.28515625" style="61" customWidth="1"/>
-    <col min="20" max="20" width="17.7109375" style="61" customWidth="1"/>
-    <col min="21" max="21" width="20.42578125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="11" style="49" customWidth="1"/>
-    <col min="23" max="23" width="10.42578125" style="49" customWidth="1"/>
-    <col min="24" max="24" width="23.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="15.140625" style="49" customWidth="1"/>
-    <col min="26" max="26" width="26.85546875" style="1" customWidth="1"/>
-    <col min="27" max="27" width="20.42578125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="11" style="49" customWidth="1"/>
-    <col min="29" max="29" width="10.42578125" style="49" customWidth="1"/>
-    <col min="30" max="30" width="23.85546875" style="1" customWidth="1"/>
-    <col min="31" max="31" width="15.140625" style="49" customWidth="1"/>
-    <col min="32" max="45" width="26.85546875" style="1" customWidth="1"/>
-    <col min="46" max="46" width="9.140625" style="1"/>
-    <col min="47" max="47" width="9.140625" style="49"/>
-    <col min="48" max="48" width="10.42578125" style="1" customWidth="1"/>
-    <col min="49" max="49" width="19" style="49" customWidth="1"/>
-    <col min="50" max="50" width="19.140625" style="49" customWidth="1"/>
-    <col min="51" max="51" width="10.42578125" style="1" customWidth="1"/>
-    <col min="52" max="52" width="11.42578125" style="49" customWidth="1"/>
-    <col min="53" max="53" width="26.85546875" style="1" customWidth="1"/>
-    <col min="54" max="54" width="9.140625" style="1"/>
-    <col min="55" max="55" width="9.140625" style="49"/>
-    <col min="56" max="56" width="10.42578125" style="1" customWidth="1"/>
-    <col min="57" max="57" width="19" style="49" customWidth="1"/>
-    <col min="58" max="58" width="19.140625" style="49" customWidth="1"/>
-    <col min="59" max="59" width="10.42578125" style="1" customWidth="1"/>
-    <col min="60" max="60" width="11.42578125" style="49" customWidth="1"/>
-    <col min="61" max="61" width="15.85546875" style="61" customWidth="1"/>
-    <col min="62" max="62" width="10.42578125" style="1" customWidth="1"/>
-    <col min="63" max="64" width="9.140625" style="1"/>
-    <col min="65" max="65" width="15.28515625" style="1" customWidth="1"/>
-    <col min="66" max="66" width="22.7109375" style="1"/>
-    <col min="67" max="67" width="15.28515625" style="1" customWidth="1"/>
-    <col min="68" max="68" width="13" style="1" customWidth="1"/>
-    <col min="69" max="69" width="15.42578125" style="1" customWidth="1"/>
-    <col min="70" max="70" width="22.7109375" style="1"/>
-    <col min="71" max="71" width="15.28515625" style="1" customWidth="1"/>
-    <col min="72" max="72" width="9.140625" style="1"/>
-    <col min="73" max="73" width="15.140625" style="1" customWidth="1"/>
-    <col min="74" max="74" width="20.140625" style="1" customWidth="1"/>
-    <col min="75" max="75" width="15.28515625" style="1" customWidth="1"/>
-    <col min="76" max="76" width="12.85546875" style="1" customWidth="1"/>
-    <col min="77" max="77" width="15.140625" style="1" customWidth="1"/>
-    <col min="78" max="78" width="20.140625" style="1" customWidth="1"/>
-    <col min="79" max="79" width="15.28515625" style="1" customWidth="1"/>
-    <col min="80" max="80" width="12.85546875" style="1" customWidth="1"/>
-    <col min="81" max="81" width="15.140625" style="1" customWidth="1"/>
-    <col min="82" max="82" width="20.140625" style="1" customWidth="1"/>
-    <col min="83" max="83" width="15.28515625" style="1" customWidth="1"/>
-    <col min="84" max="84" width="12.85546875" style="1" customWidth="1"/>
-    <col min="85" max="85" width="9.140625" style="1"/>
-    <col min="86" max="86" width="11.42578125" style="1" customWidth="1"/>
-    <col min="87" max="87" width="15.28515625" style="1" customWidth="1"/>
-    <col min="88" max="89" width="9.140625" style="1"/>
-    <col min="90" max="90" width="11.42578125" style="1" customWidth="1"/>
-    <col min="91" max="91" width="15.28515625" style="1" customWidth="1"/>
-    <col min="92" max="94" width="9.140625" style="1"/>
-    <col min="95" max="95" width="15.28515625" style="1" customWidth="1"/>
-    <col min="96" max="98" width="9.140625" style="1"/>
-    <col min="99" max="99" width="15.28515625" style="1" customWidth="1"/>
-    <col min="100" max="102" width="9.140625" style="1"/>
-    <col min="103" max="103" width="15.28515625" style="1" customWidth="1"/>
-    <col min="104" max="104" width="9.140625" style="1"/>
-    <col min="105" max="105" width="11.42578125" style="1" customWidth="1"/>
-    <col min="106" max="106" width="12.28515625" style="1" customWidth="1"/>
-    <col min="107" max="109" width="13.42578125" style="1" customWidth="1"/>
-    <col min="110" max="111" width="10.85546875" style="1" customWidth="1"/>
-    <col min="112" max="112" width="15.42578125" style="1" customWidth="1"/>
-    <col min="113" max="113" width="9.28515625" style="1"/>
-    <col min="114" max="114" width="17.7109375" style="1" customWidth="1"/>
-    <col min="115" max="115" width="17" style="1" customWidth="1"/>
-    <col min="116" max="116" width="17.7109375" style="1" customWidth="1"/>
-    <col min="117" max="117" width="12.28515625" style="1" customWidth="1"/>
-    <col min="118" max="118" width="17.7109375" style="1" customWidth="1"/>
-    <col min="119" max="119" width="11.7109375" style="1" customWidth="1"/>
-    <col min="120" max="120" width="17.7109375" style="1" customWidth="1"/>
-    <col min="121" max="121" width="16" style="1" customWidth="1"/>
-    <col min="122" max="122" width="17.7109375" style="1" customWidth="1"/>
-    <col min="123" max="123" width="9.140625" style="1"/>
-    <col min="124" max="124" width="17.7109375" style="1" customWidth="1"/>
-    <col min="125" max="125" width="12" customWidth="1"/>
-    <col min="126" max="126" width="17.7109375" style="1" customWidth="1"/>
-    <col min="127" max="127" width="11.85546875" style="1" customWidth="1"/>
-    <col min="128" max="128" width="17.7109375" style="1" customWidth="1"/>
-    <col min="129" max="129" width="11.85546875" style="1" customWidth="1"/>
-    <col min="130" max="130" width="17.7109375" style="1" customWidth="1"/>
-    <col min="131" max="131" width="11.85546875" style="1" customWidth="1"/>
-    <col min="132" max="132" width="17.7109375" style="1" customWidth="1"/>
-    <col min="133" max="133" width="11.85546875" style="1" customWidth="1"/>
-    <col min="134" max="134" width="17.7109375" style="1" customWidth="1"/>
-    <col min="135" max="135" width="14.85546875" style="1" customWidth="1"/>
-    <col min="136" max="136" width="17.7109375" style="1" customWidth="1"/>
-    <col min="137" max="137" width="12.28515625" style="1" customWidth="1"/>
-    <col min="138" max="138" width="17.7109375" style="1" customWidth="1"/>
-    <col min="139" max="139" width="9.140625" style="1"/>
-    <col min="140" max="140" width="17.7109375" style="1" customWidth="1"/>
-    <col min="141" max="141" width="9.140625" style="1"/>
-    <col min="142" max="142" width="17.7109375" style="1" customWidth="1"/>
-    <col min="143" max="143" width="18.42578125" style="1" customWidth="1"/>
-    <col min="144" max="144" width="17.7109375" style="1" customWidth="1"/>
-    <col min="145" max="145" width="10.140625" style="1" customWidth="1"/>
-    <col min="146" max="146" width="17.7109375" style="1" customWidth="1"/>
-    <col min="147" max="1134" width="9.28515625" style="1"/>
+    <col min="1" max="1" width="13.15625" style="31" customWidth="1"/>
+    <col min="2" max="2" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="11.68359375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.68359375" style="63" customWidth="1"/>
+    <col min="5" max="5" width="10.83984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.68359375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.41796875" customWidth="1"/>
+    <col min="8" max="8" width="30.15625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.41796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.41796875" customWidth="1"/>
+    <col min="11" max="11" width="17.68359375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.578125" style="45" customWidth="1"/>
+    <col min="13" max="13" width="14.26171875" style="1" customWidth="1"/>
+    <col min="14" max="16" width="14.26171875" style="63" customWidth="1"/>
+    <col min="17" max="17" width="17.68359375" style="63" customWidth="1"/>
+    <col min="18" max="20" width="14.26171875" style="63" customWidth="1"/>
+    <col min="21" max="21" width="17.68359375" style="63" customWidth="1"/>
+    <col min="22" max="22" width="20.41796875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11" style="50" customWidth="1"/>
+    <col min="24" max="24" width="10.578125" style="50" customWidth="1"/>
+    <col min="25" max="25" width="23.83984375" style="1" customWidth="1"/>
+    <col min="26" max="26" width="15.15625" style="50" customWidth="1"/>
+    <col min="27" max="27" width="26.83984375" style="1" customWidth="1"/>
+    <col min="28" max="28" width="20.41796875" style="1" customWidth="1"/>
+    <col min="29" max="29" width="11" style="50" customWidth="1"/>
+    <col min="30" max="30" width="10.578125" style="50" customWidth="1"/>
+    <col min="31" max="31" width="23.83984375" style="1" customWidth="1"/>
+    <col min="32" max="32" width="15.15625" style="50" customWidth="1"/>
+    <col min="33" max="46" width="26.83984375" style="1" customWidth="1"/>
+    <col min="47" max="47" width="9.15625" style="1"/>
+    <col min="48" max="48" width="9.15625" style="50"/>
+    <col min="49" max="49" width="10.41796875" style="1" customWidth="1"/>
+    <col min="50" max="50" width="19" style="50" customWidth="1"/>
+    <col min="51" max="51" width="19.15625" style="50" customWidth="1"/>
+    <col min="52" max="52" width="10.41796875" style="1" customWidth="1"/>
+    <col min="53" max="53" width="11.41796875" style="50" customWidth="1"/>
+    <col min="54" max="54" width="26.83984375" style="1" customWidth="1"/>
+    <col min="55" max="55" width="9.15625" style="1"/>
+    <col min="56" max="56" width="9.15625" style="50"/>
+    <col min="57" max="57" width="10.41796875" style="1" customWidth="1"/>
+    <col min="58" max="58" width="19" style="50" customWidth="1"/>
+    <col min="59" max="59" width="19.15625" style="50" customWidth="1"/>
+    <col min="60" max="60" width="10.41796875" style="1" customWidth="1"/>
+    <col min="61" max="61" width="11.41796875" style="50" customWidth="1"/>
+    <col min="62" max="62" width="15.83984375" style="63" customWidth="1"/>
+    <col min="63" max="63" width="10.41796875" style="1" customWidth="1"/>
+    <col min="64" max="65" width="9.15625" style="1"/>
+    <col min="66" max="66" width="15.26171875" style="1" customWidth="1"/>
+    <col min="67" max="67" width="22.68359375" style="1"/>
+    <col min="68" max="68" width="15.26171875" style="1" customWidth="1"/>
+    <col min="69" max="69" width="13" style="1" customWidth="1"/>
+    <col min="70" max="70" width="15.41796875" style="1" customWidth="1"/>
+    <col min="71" max="71" width="22.68359375" style="1"/>
+    <col min="72" max="72" width="15.26171875" style="1" customWidth="1"/>
+    <col min="73" max="73" width="9.15625" style="1"/>
+    <col min="74" max="74" width="15.15625" style="1" customWidth="1"/>
+    <col min="75" max="75" width="20.15625" style="1" customWidth="1"/>
+    <col min="76" max="76" width="15.26171875" style="1" customWidth="1"/>
+    <col min="77" max="77" width="12.83984375" style="1" customWidth="1"/>
+    <col min="78" max="78" width="15.15625" style="1" customWidth="1"/>
+    <col min="79" max="79" width="20.15625" style="1" customWidth="1"/>
+    <col min="80" max="80" width="15.26171875" style="1" customWidth="1"/>
+    <col min="81" max="81" width="12.83984375" style="1" customWidth="1"/>
+    <col min="82" max="82" width="15.15625" style="1" customWidth="1"/>
+    <col min="83" max="83" width="20.15625" style="1" customWidth="1"/>
+    <col min="84" max="84" width="15.26171875" style="1" customWidth="1"/>
+    <col min="85" max="85" width="12.83984375" style="1" customWidth="1"/>
+    <col min="86" max="86" width="9.15625" style="1"/>
+    <col min="87" max="87" width="11.41796875" style="1" customWidth="1"/>
+    <col min="88" max="88" width="15.26171875" style="1" customWidth="1"/>
+    <col min="89" max="90" width="9.15625" style="1"/>
+    <col min="91" max="91" width="11.41796875" style="1" customWidth="1"/>
+    <col min="92" max="92" width="15.26171875" style="1" customWidth="1"/>
+    <col min="93" max="95" width="9.15625" style="1"/>
+    <col min="96" max="96" width="15.26171875" style="1" customWidth="1"/>
+    <col min="97" max="99" width="9.15625" style="1"/>
+    <col min="100" max="100" width="15.26171875" style="1" customWidth="1"/>
+    <col min="101" max="103" width="9.15625" style="1"/>
+    <col min="104" max="104" width="15.26171875" style="1" customWidth="1"/>
+    <col min="105" max="105" width="9.15625" style="1"/>
+    <col min="106" max="106" width="11.578125" style="1" customWidth="1"/>
+    <col min="107" max="107" width="12.26171875" style="1" customWidth="1"/>
+    <col min="108" max="110" width="13.578125" style="1" customWidth="1"/>
+    <col min="111" max="112" width="10.83984375" style="1" customWidth="1"/>
+    <col min="113" max="113" width="15.41796875" style="1" customWidth="1"/>
+    <col min="114" max="114" width="9.26171875" style="1"/>
+    <col min="115" max="115" width="17.68359375" style="1" customWidth="1"/>
+    <col min="116" max="116" width="17" style="1" customWidth="1"/>
+    <col min="117" max="117" width="17.68359375" style="1" customWidth="1"/>
+    <col min="118" max="118" width="12.26171875" style="1" customWidth="1"/>
+    <col min="119" max="119" width="17.68359375" style="1" customWidth="1"/>
+    <col min="120" max="120" width="11.68359375" style="1" customWidth="1"/>
+    <col min="121" max="121" width="17.68359375" style="1" customWidth="1"/>
+    <col min="122" max="122" width="16" style="1" customWidth="1"/>
+    <col min="123" max="123" width="17.68359375" style="1" customWidth="1"/>
+    <col min="124" max="124" width="9.15625" style="1"/>
+    <col min="125" max="125" width="17.68359375" style="1" customWidth="1"/>
+    <col min="126" max="126" width="12" customWidth="1"/>
+    <col min="127" max="127" width="17.68359375" style="1" customWidth="1"/>
+    <col min="128" max="128" width="11.83984375" style="1" customWidth="1"/>
+    <col min="129" max="129" width="17.68359375" style="1" customWidth="1"/>
+    <col min="130" max="130" width="11.83984375" style="1" customWidth="1"/>
+    <col min="131" max="131" width="17.68359375" style="1" customWidth="1"/>
+    <col min="132" max="132" width="11.83984375" style="1" customWidth="1"/>
+    <col min="133" max="133" width="17.68359375" style="1" customWidth="1"/>
+    <col min="134" max="134" width="11.83984375" style="1" customWidth="1"/>
+    <col min="135" max="135" width="17.68359375" style="1" customWidth="1"/>
+    <col min="136" max="136" width="14.83984375" style="1" customWidth="1"/>
+    <col min="137" max="137" width="17.68359375" style="1" customWidth="1"/>
+    <col min="138" max="138" width="12.26171875" style="1" customWidth="1"/>
+    <col min="139" max="139" width="17.68359375" style="1" customWidth="1"/>
+    <col min="140" max="140" width="9.15625" style="1"/>
+    <col min="141" max="141" width="17.68359375" style="1" customWidth="1"/>
+    <col min="142" max="142" width="9.15625" style="1"/>
+    <col min="143" max="143" width="17.68359375" style="1" customWidth="1"/>
+    <col min="144" max="144" width="18.41796875" style="1" customWidth="1"/>
+    <col min="145" max="145" width="17.68359375" style="1" customWidth="1"/>
+    <col min="146" max="146" width="10.15625" style="1" customWidth="1"/>
+    <col min="147" max="147" width="17.68359375" style="1" customWidth="1"/>
+    <col min="148" max="1135" width="9.26171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:146" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:147" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="31" t="s">
-        <v>394</v>
-      </c>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
+        <v>397</v>
+      </c>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="64"/>
+      <c r="T1" s="64"/>
     </row>
-    <row r="2" spans="1:146" s="1" customFormat="1" ht="64.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:147" s="1" customFormat="1" ht="51.9" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="L2" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N2" s="69" t="s">
+        <v>377</v>
+      </c>
+      <c r="O2" s="69" t="s">
+        <v>377</v>
+      </c>
+      <c r="P2" s="69" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q2" s="71" t="s">
+        <v>377</v>
+      </c>
+      <c r="R2" s="69" t="s">
+        <v>377</v>
+      </c>
+      <c r="S2" s="69" t="s">
+        <v>377</v>
+      </c>
+      <c r="T2" s="69" t="s">
+        <v>377</v>
+      </c>
+      <c r="U2" s="71" t="s">
+        <v>377</v>
+      </c>
+      <c r="V2" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="W2" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="X2" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="Y2" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="Z2" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="AA2" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="K2" s="41" t="s">
-        <v>96</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="M2" s="67" t="s">
-        <v>374</v>
-      </c>
-      <c r="N2" s="67" t="s">
-        <v>374</v>
-      </c>
-      <c r="O2" s="67" t="s">
-        <v>374</v>
-      </c>
-      <c r="P2" s="69" t="s">
-        <v>374</v>
-      </c>
-      <c r="Q2" s="67" t="s">
-        <v>374</v>
-      </c>
-      <c r="R2" s="67" t="s">
-        <v>374</v>
-      </c>
-      <c r="S2" s="67" t="s">
-        <v>374</v>
-      </c>
-      <c r="T2" s="69" t="s">
-        <v>374</v>
-      </c>
-      <c r="U2" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="V2" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="W2" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="X2" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y2" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z2" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="AA2" s="18" t="s">
-        <v>344</v>
-      </c>
-      <c r="AB2" s="54" t="s">
-        <v>344</v>
-      </c>
-      <c r="AC2" s="54" t="s">
-        <v>344</v>
-      </c>
-      <c r="AD2" s="18" t="s">
-        <v>345</v>
-      </c>
-      <c r="AE2" s="54" t="s">
-        <v>344</v>
-      </c>
-      <c r="AF2" s="18" t="s">
-        <v>344</v>
-      </c>
-      <c r="AG2" s="12" t="s">
-        <v>82</v>
+      <c r="AB2" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="AC2" s="55" t="s">
+        <v>347</v>
+      </c>
+      <c r="AD2" s="55" t="s">
+        <v>347</v>
+      </c>
+      <c r="AE2" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="AF2" s="55" t="s">
+        <v>347</v>
+      </c>
+      <c r="AG2" s="18" t="s">
+        <v>347</v>
       </c>
       <c r="AH2" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AI2" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AJ2" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AK2" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AL2" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AM2" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AN2" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AO2" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AP2" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AQ2" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AR2" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="AS2" s="20" t="s">
-        <v>29</v>
+        <v>83</v>
+      </c>
+      <c r="AS2" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="AT2" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="AU2" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="AV2" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="AW2" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="AX2" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="AY2" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="AZ2" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="BA2" s="20" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="AU2" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="AV2" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="AW2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="AX2" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="AY2" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="AZ2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="BA2" s="51" t="s">
+        <v>30</v>
       </c>
       <c r="BB2" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="BC2" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="BD2" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="BE2" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="BF2" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="BG2" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="BH2" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="BI2" s="70" t="s">
-        <v>40</v>
-      </c>
-      <c r="BJ2" s="22" t="s">
-        <v>40</v>
+        <v>30</v>
+      </c>
+      <c r="BC2" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="BD2" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="BE2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="BF2" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="BG2" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="BH2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="BI2" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="BJ2" s="72" t="s">
+        <v>41</v>
       </c>
       <c r="BK2" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="BL2" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="BM2" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="BL2" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="BM2" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="BN2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="BN2" s="19" t="s">
+      <c r="BO2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BO2" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="BP2" s="19" t="s">
+      <c r="BP2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BQ2" s="19" t="s">
@@ -2524,10 +2553,10 @@
       <c r="BR2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BS2" s="47" t="s">
+      <c r="BS2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BT2" s="19" t="s">
+      <c r="BT2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BU2" s="19" t="s">
@@ -2536,10 +2565,10 @@
       <c r="BV2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BW2" s="47" t="s">
+      <c r="BW2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="BX2" s="19" t="s">
+      <c r="BX2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="BY2" s="19" t="s">
@@ -2548,10 +2577,10 @@
       <c r="BZ2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CA2" s="47" t="s">
+      <c r="CA2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CB2" s="19" t="s">
+      <c r="CB2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="CC2" s="19" t="s">
@@ -2560,10 +2589,10 @@
       <c r="CD2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CE2" s="47" t="s">
+      <c r="CE2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CF2" s="19" t="s">
+      <c r="CF2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="CG2" s="19" t="s">
@@ -2572,10 +2601,10 @@
       <c r="CH2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CI2" s="47" t="s">
+      <c r="CI2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CJ2" s="19" t="s">
+      <c r="CJ2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="CK2" s="19" t="s">
@@ -2584,10 +2613,10 @@
       <c r="CL2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CM2" s="47" t="s">
+      <c r="CM2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CN2" s="19" t="s">
+      <c r="CN2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="CO2" s="19" t="s">
@@ -2596,10 +2625,10 @@
       <c r="CP2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CQ2" s="47" t="s">
+      <c r="CQ2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CR2" s="19" t="s">
+      <c r="CR2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="CS2" s="19" t="s">
@@ -2608,10 +2637,10 @@
       <c r="CT2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CU2" s="47" t="s">
+      <c r="CU2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CV2" s="19" t="s">
+      <c r="CV2" s="48" t="s">
         <v>1</v>
       </c>
       <c r="CW2" s="19" t="s">
@@ -2620,1490 +2649,1502 @@
       <c r="CX2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CY2" s="47" t="s">
+      <c r="CY2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="CZ2" s="19" t="s">
+      <c r="CZ2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="DA2" s="21" t="s">
-        <v>117</v>
+      <c r="DA2" s="19" t="s">
+        <v>1</v>
       </c>
       <c r="DB2" s="21" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="DC2" s="21" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="DD2" s="21" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="DE2" s="21" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="DF2" s="21" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="DG2" s="21" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="DH2" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="DI2" s="29" t="s">
-        <v>64</v>
+        <v>120</v>
+      </c>
+      <c r="DI2" s="21" t="s">
+        <v>120</v>
       </c>
       <c r="DJ2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="DK2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="DL2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="DM2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="DN2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="DO2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="DP2" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="DQ2" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="DR2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="DQ2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="DR2" s="28" t="s">
+        <v>65</v>
       </c>
       <c r="DS2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="DT2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="DU2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="DV2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="DW2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="DX2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="DY2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="DZ2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="EA2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="EB2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="EC2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="ED2" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="EE2" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="EF2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="EE2" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="EF2" s="30" t="s">
+        <v>65</v>
       </c>
       <c r="EG2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="EH2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="EI2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="EJ2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="EK2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="EL2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="EM2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="EN2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="EO2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="EP2" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="EQ2" s="29" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:146" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:147" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="34" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L3" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="70" t="s">
+        <v>378</v>
+      </c>
+      <c r="O3" s="70" t="s">
+        <v>379</v>
+      </c>
+      <c r="P3" s="70" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q3" s="70" t="s">
+        <v>392</v>
+      </c>
+      <c r="R3" s="70" t="s">
+        <v>393</v>
+      </c>
+      <c r="S3" s="70" t="s">
+        <v>394</v>
+      </c>
+      <c r="T3" s="70" t="s">
+        <v>395</v>
+      </c>
+      <c r="U3" s="70" t="s">
+        <v>396</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="W3" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="X3" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y3" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z3" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA3" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC3" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD3" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE3" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF3" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG3" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH3" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AK3" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AL3" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AM3" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN3" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AQ3" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AR3" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS3" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT3" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="AU3" s="49" t="s">
+        <v>203</v>
+      </c>
+      <c r="AV3" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="AW3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AX3" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="AY3" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ3" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="BA3" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="BB3" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="BC3" s="49" t="s">
+        <v>203</v>
+      </c>
+      <c r="BD3" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="BE3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="BF3" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="BG3" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="BH3" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="BI3" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="BJ3" s="73" t="s">
+        <v>404</v>
+      </c>
+      <c r="BK3" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="BL3" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="BM3" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="BN3" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="BO3" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="BP3" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="BQ3" s="27" t="s">
+        <v>287</v>
+      </c>
+      <c r="BR3" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="BS3" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="BT3" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="BU3" s="27" t="s">
+        <v>288</v>
+      </c>
+      <c r="BV3" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="BW3" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="BX3" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="BY3" s="27" t="s">
+        <v>312</v>
+      </c>
+      <c r="BZ3" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="CA3" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="CB3" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="CC3" s="27" t="s">
+        <v>312</v>
+      </c>
+      <c r="CD3" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="CE3" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="CF3" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="CG3" s="27" t="s">
+        <v>312</v>
+      </c>
+      <c r="CH3" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="CI3" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="CJ3" s="27" t="s">
+        <v>279</v>
+      </c>
+      <c r="CK3" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="CL3" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="CM3" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="CN3" s="27" t="s">
+        <v>279</v>
+      </c>
+      <c r="CO3" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="CP3" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="CQ3" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="CR3" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="CS3" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="CT3" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="CU3" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="CV3" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="CW3" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="CX3" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="CY3" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="CZ3" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="DA3" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="DB3" s="62" t="s">
+        <v>163</v>
+      </c>
+      <c r="DC3" s="62" t="s">
         <v>398</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="DD3" s="62" t="s">
         <v>399</v>
       </c>
-      <c r="D3" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="K3" s="42" t="s">
-        <v>159</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="68" t="s">
-        <v>375</v>
-      </c>
-      <c r="N3" s="68" t="s">
-        <v>376</v>
-      </c>
-      <c r="O3" s="68" t="s">
-        <v>377</v>
-      </c>
-      <c r="P3" s="68" t="s">
-        <v>389</v>
-      </c>
-      <c r="Q3" s="68" t="s">
-        <v>390</v>
-      </c>
-      <c r="R3" s="68" t="s">
-        <v>391</v>
-      </c>
-      <c r="S3" s="68" t="s">
-        <v>392</v>
-      </c>
-      <c r="T3" s="68" t="s">
-        <v>393</v>
-      </c>
-      <c r="U3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="V3" s="55" t="s">
-        <v>16</v>
-      </c>
-      <c r="W3" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="X3" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y3" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z3" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB3" s="55" t="s">
-        <v>16</v>
-      </c>
-      <c r="AC3" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="AD3" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="AE3" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF3" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="AG3" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="AJ3" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK3" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="AL3" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="AM3" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="AN3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="AP3" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="AQ3" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="AR3" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="AS3" s="48" t="s">
-        <v>197</v>
-      </c>
-      <c r="AT3" s="48" t="s">
-        <v>200</v>
-      </c>
-      <c r="AU3" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="AV3" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="AW3" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="AX3" s="51" t="s">
-        <v>91</v>
-      </c>
-      <c r="AY3" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="AZ3" s="51" t="s">
-        <v>92</v>
-      </c>
-      <c r="BA3" s="48" t="s">
-        <v>197</v>
-      </c>
-      <c r="BB3" s="48" t="s">
-        <v>200</v>
-      </c>
-      <c r="BC3" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="BD3" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="BE3" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="BF3" s="51" t="s">
-        <v>91</v>
-      </c>
-      <c r="BG3" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="BH3" s="51" t="s">
-        <v>92</v>
-      </c>
-      <c r="BI3" s="71" t="s">
-        <v>401</v>
-      </c>
-      <c r="BJ3" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="BK3" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="BL3" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="BM3" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="BN3" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="BO3" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="BP3" s="27" t="s">
-        <v>284</v>
-      </c>
-      <c r="BQ3" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="BR3" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="BS3" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="BT3" s="27" t="s">
-        <v>285</v>
-      </c>
-      <c r="BU3" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="BV3" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="BW3" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="BX3" s="27" t="s">
-        <v>309</v>
-      </c>
-      <c r="BY3" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="BZ3" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="CA3" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="CB3" s="27" t="s">
-        <v>309</v>
-      </c>
-      <c r="CC3" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="CD3" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="CE3" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="CF3" s="27" t="s">
-        <v>309</v>
-      </c>
-      <c r="CG3" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="CH3" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="CI3" s="27" t="s">
-        <v>276</v>
-      </c>
-      <c r="CJ3" s="27" t="s">
-        <v>278</v>
-      </c>
-      <c r="CK3" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="CL3" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="CM3" s="27" t="s">
-        <v>276</v>
-      </c>
-      <c r="CN3" s="27" t="s">
-        <v>278</v>
-      </c>
-      <c r="CO3" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="CP3" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="CQ3" s="27" t="s">
-        <v>280</v>
-      </c>
-      <c r="CR3" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="CS3" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="CT3" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="CU3" s="27" t="s">
-        <v>280</v>
-      </c>
-      <c r="CV3" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="CW3" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="CX3" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="CY3" s="27" t="s">
-        <v>280</v>
-      </c>
-      <c r="CZ3" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="DA3" s="60" t="s">
-        <v>160</v>
-      </c>
-      <c r="DB3" s="60" t="s">
-        <v>395</v>
-      </c>
-      <c r="DC3" s="60" t="s">
-        <v>396</v>
-      </c>
-      <c r="DD3" s="60" t="s">
-        <v>176</v>
-      </c>
-      <c r="DE3" s="60" t="s">
-        <v>160</v>
-      </c>
-      <c r="DF3" s="60" t="s">
-        <v>395</v>
-      </c>
-      <c r="DG3" s="60" t="s">
-        <v>396</v>
-      </c>
-      <c r="DH3" s="60" t="s">
-        <v>176</v>
-      </c>
-      <c r="DI3" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="DJ3" s="57" t="s">
-        <v>236</v>
-      </c>
-      <c r="DK3" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="DL3" s="57" t="s">
-        <v>234</v>
-      </c>
-      <c r="DM3" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="DN3" s="57" t="s">
-        <v>232</v>
-      </c>
-      <c r="DO3" s="26" t="s">
+      <c r="DE3" s="62" t="s">
+        <v>179</v>
+      </c>
+      <c r="DF3" s="62" t="s">
+        <v>163</v>
+      </c>
+      <c r="DG3" s="62" t="s">
+        <v>398</v>
+      </c>
+      <c r="DH3" s="62" t="s">
+        <v>399</v>
+      </c>
+      <c r="DI3" s="62" t="s">
+        <v>179</v>
+      </c>
+      <c r="DJ3" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="DP3" s="57" t="s">
-        <v>230</v>
-      </c>
-      <c r="DQ3" s="26" t="s">
+      <c r="DK3" s="59" t="s">
+        <v>239</v>
+      </c>
+      <c r="DL3" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="DR3" s="57" t="s">
-        <v>228</v>
-      </c>
-      <c r="DS3" s="26" t="s">
+      <c r="DM3" s="59" t="s">
+        <v>237</v>
+      </c>
+      <c r="DN3" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="DT3" s="57" t="s">
-        <v>226</v>
-      </c>
-      <c r="DU3" s="26" t="s">
+      <c r="DO3" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="DP3" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="DV3" s="57" t="s">
-        <v>224</v>
-      </c>
-      <c r="DW3" s="26" t="s">
+      <c r="DQ3" s="59" t="s">
+        <v>233</v>
+      </c>
+      <c r="DR3" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="DX3" s="57" t="s">
-        <v>222</v>
-      </c>
-      <c r="DY3" s="26" t="s">
+      <c r="DS3" s="59" t="s">
+        <v>231</v>
+      </c>
+      <c r="DT3" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="DZ3" s="57" t="s">
-        <v>220</v>
-      </c>
-      <c r="EA3" s="26" t="s">
+      <c r="DU3" s="59" t="s">
+        <v>229</v>
+      </c>
+      <c r="DV3" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="DW3" s="59" t="s">
+        <v>227</v>
+      </c>
+      <c r="DX3" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="EB3" s="57" t="s">
-        <v>218</v>
-      </c>
-      <c r="EC3" s="26" t="s">
+      <c r="DY3" s="59" t="s">
+        <v>225</v>
+      </c>
+      <c r="DZ3" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="ED3" s="57" t="s">
+      <c r="EA3" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="EB3" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="EC3" s="59" t="s">
+        <v>221</v>
+      </c>
+      <c r="ED3" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="EE3" s="59" t="s">
+        <v>219</v>
+      </c>
+      <c r="EF3" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="EG3" s="59" t="s">
+        <v>217</v>
+      </c>
+      <c r="EH3" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="EI3" s="59" t="s">
         <v>216</v>
       </c>
-      <c r="EE3" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="EF3" s="57" t="s">
-        <v>214</v>
-      </c>
-      <c r="EG3" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="EH3" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="EI3" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="EJ3" s="57" t="s">
+      <c r="EJ3" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="EK3" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="EL3" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="EM3" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="EN3" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="EO3" s="59" t="s">
         <v>209</v>
       </c>
-      <c r="EK3" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="EL3" s="57" t="s">
-        <v>208</v>
-      </c>
-      <c r="EM3" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="EN3" s="57" t="s">
-        <v>206</v>
-      </c>
-      <c r="EO3" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="EP3" s="57" t="s">
-        <v>204</v>
+      <c r="EP3" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="EQ3" s="59" t="s">
+        <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:146" s="58" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:147" s="60" customFormat="1" ht="56.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="64" t="s">
-        <v>400</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="38" t="s">
+      <c r="B4" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>403</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>204</v>
+      </c>
+      <c r="K4" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="L4" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="M4" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="66" t="s">
+        <v>381</v>
+      </c>
+      <c r="O4" s="66" t="s">
+        <v>382</v>
+      </c>
+      <c r="P4" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q4" s="68" t="s">
+        <v>249</v>
+      </c>
+      <c r="R4" s="66" t="s">
+        <v>383</v>
+      </c>
+      <c r="S4" s="66" t="s">
+        <v>384</v>
+      </c>
+      <c r="T4" s="66" t="s">
+        <v>385</v>
+      </c>
+      <c r="U4" s="68" t="s">
+        <v>386</v>
+      </c>
+      <c r="V4" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="W4" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="X4" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y4" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z4" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA4" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB4" s="38" t="s">
+        <v>335</v>
+      </c>
+      <c r="AC4" s="40" t="s">
+        <v>338</v>
+      </c>
+      <c r="AD4" s="40" t="s">
+        <v>339</v>
+      </c>
+      <c r="AE4" s="38" t="s">
+        <v>341</v>
+      </c>
+      <c r="AF4" s="40" t="s">
+        <v>343</v>
+      </c>
+      <c r="AG4" s="38" t="s">
+        <v>345</v>
+      </c>
+      <c r="AH4" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI4" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="AJ4" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK4" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="AL4" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM4" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN4" s="38" t="s">
+        <v>350</v>
+      </c>
+      <c r="AO4" s="38" t="s">
+        <v>351</v>
+      </c>
+      <c r="AP4" s="38" t="s">
+        <v>353</v>
+      </c>
+      <c r="AQ4" s="38" t="s">
+        <v>355</v>
+      </c>
+      <c r="AR4" s="38" t="s">
+        <v>357</v>
+      </c>
+      <c r="AS4" s="61" t="s">
+        <v>359</v>
+      </c>
+      <c r="AT4" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="AU4" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="AV4" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="AW4" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="AX4" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="AY4" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="40" t="s">
-        <v>101</v>
-      </c>
-      <c r="G4" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="38" t="s">
-        <v>201</v>
-      </c>
-      <c r="J4" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="K4" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="L4" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="M4" s="64" t="s">
-        <v>378</v>
-      </c>
-      <c r="N4" s="64" t="s">
-        <v>379</v>
-      </c>
-      <c r="O4" s="66" t="s">
-        <v>59</v>
-      </c>
-      <c r="P4" s="66" t="s">
-        <v>246</v>
-      </c>
-      <c r="Q4" s="64" t="s">
-        <v>380</v>
-      </c>
-      <c r="R4" s="64" t="s">
-        <v>381</v>
-      </c>
-      <c r="S4" s="64" t="s">
-        <v>382</v>
-      </c>
-      <c r="T4" s="66" t="s">
-        <v>383</v>
-      </c>
-      <c r="U4" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="V4" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="W4" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="X4" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y4" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z4" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA4" s="38" t="s">
-        <v>332</v>
-      </c>
-      <c r="AB4" s="39" t="s">
-        <v>335</v>
-      </c>
-      <c r="AC4" s="39" t="s">
-        <v>336</v>
-      </c>
-      <c r="AD4" s="38" t="s">
-        <v>338</v>
-      </c>
-      <c r="AE4" s="39" t="s">
-        <v>340</v>
-      </c>
-      <c r="AF4" s="38" t="s">
-        <v>342</v>
-      </c>
-      <c r="AG4" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="AH4" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="AI4" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="AJ4" s="38" t="s">
-        <v>128</v>
-      </c>
-      <c r="AK4" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="AL4" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM4" s="38" t="s">
-        <v>347</v>
-      </c>
-      <c r="AN4" s="38" t="s">
-        <v>348</v>
-      </c>
-      <c r="AO4" s="38" t="s">
-        <v>350</v>
-      </c>
-      <c r="AP4" s="38" t="s">
-        <v>352</v>
-      </c>
-      <c r="AQ4" s="38" t="s">
-        <v>354</v>
-      </c>
-      <c r="AR4" s="59" t="s">
-        <v>356</v>
-      </c>
-      <c r="AS4" s="38" t="s">
+      <c r="AZ4" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="BA4" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="BB4" s="38" t="s">
+        <v>361</v>
+      </c>
+      <c r="BC4" s="38" t="s">
+        <v>363</v>
+      </c>
+      <c r="BD4" s="40" t="s">
+        <v>365</v>
+      </c>
+      <c r="BE4" s="38" t="s">
+        <v>368</v>
+      </c>
+      <c r="BF4" s="40" t="s">
+        <v>369</v>
+      </c>
+      <c r="BG4" s="40" t="s">
+        <v>371</v>
+      </c>
+      <c r="BH4" s="38" t="s">
+        <v>373</v>
+      </c>
+      <c r="BI4" s="40" t="s">
+        <v>375</v>
+      </c>
+      <c r="BJ4" s="74" t="s">
+        <v>405</v>
+      </c>
+      <c r="BK4" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="BL4" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="BM4" s="38" t="s">
+        <v>206</v>
+      </c>
+      <c r="BN4" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="BO4" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="BP4" s="38" t="s">
+        <v>260</v>
+      </c>
+      <c r="BQ4" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="BR4" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="BS4" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="BT4" s="38" t="s">
+        <v>274</v>
+      </c>
+      <c r="BU4" s="38" t="s">
+        <v>184</v>
+      </c>
+      <c r="BV4" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="BW4" s="38" t="s">
+        <v>186</v>
+      </c>
+      <c r="BX4" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="BY4" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="BZ4" s="38" t="s">
+        <v>313</v>
+      </c>
+      <c r="CA4" s="38" t="s">
+        <v>315</v>
+      </c>
+      <c r="CB4" s="38" t="s">
+        <v>317</v>
+      </c>
+      <c r="CC4" s="38" t="s">
+        <v>319</v>
+      </c>
+      <c r="CD4" s="38" t="s">
+        <v>321</v>
+      </c>
+      <c r="CE4" s="38" t="s">
+        <v>323</v>
+      </c>
+      <c r="CF4" s="38" t="s">
+        <v>325</v>
+      </c>
+      <c r="CG4" s="38" t="s">
+        <v>327</v>
+      </c>
+      <c r="CH4" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="CI4" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="AT4" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU4" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="AV4" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="AW4" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="AX4" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="AY4" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="AZ4" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="BA4" s="38" t="s">
-        <v>358</v>
-      </c>
-      <c r="BB4" s="38" t="s">
-        <v>360</v>
-      </c>
-      <c r="BC4" s="39" t="s">
-        <v>362</v>
-      </c>
-      <c r="BD4" s="38" t="s">
-        <v>365</v>
-      </c>
-      <c r="BE4" s="39" t="s">
-        <v>366</v>
-      </c>
-      <c r="BF4" s="39" t="s">
-        <v>368</v>
-      </c>
-      <c r="BG4" s="38" t="s">
-        <v>370</v>
-      </c>
-      <c r="BH4" s="39" t="s">
-        <v>372</v>
-      </c>
-      <c r="BI4" s="72" t="s">
-        <v>402</v>
-      </c>
-      <c r="BJ4" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="BK4" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="BL4" s="38" t="s">
-        <v>203</v>
-      </c>
-      <c r="BM4" s="38" t="s">
-        <v>193</v>
-      </c>
-      <c r="BN4" s="38" t="s">
-        <v>177</v>
-      </c>
-      <c r="BO4" s="38" t="s">
-        <v>257</v>
-      </c>
-      <c r="BP4" s="38" t="s">
-        <v>178</v>
-      </c>
-      <c r="BQ4" s="38" t="s">
-        <v>179</v>
-      </c>
-      <c r="BR4" s="38" t="s">
-        <v>180</v>
-      </c>
-      <c r="BS4" s="38" t="s">
-        <v>271</v>
-      </c>
-      <c r="BT4" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="BU4" s="38" t="s">
-        <v>182</v>
-      </c>
-      <c r="BV4" s="38" t="s">
-        <v>183</v>
-      </c>
-      <c r="BW4" s="38" t="s">
-        <v>274</v>
-      </c>
-      <c r="BX4" s="38" t="s">
-        <v>184</v>
-      </c>
-      <c r="BY4" s="38" t="s">
-        <v>310</v>
-      </c>
-      <c r="BZ4" s="38" t="s">
-        <v>312</v>
-      </c>
-      <c r="CA4" s="38" t="s">
-        <v>314</v>
-      </c>
-      <c r="CB4" s="38" t="s">
-        <v>316</v>
-      </c>
-      <c r="CC4" s="38" t="s">
-        <v>318</v>
-      </c>
-      <c r="CD4" s="38" t="s">
-        <v>320</v>
-      </c>
-      <c r="CE4" s="38" t="s">
-        <v>322</v>
-      </c>
-      <c r="CF4" s="38" t="s">
-        <v>324</v>
-      </c>
-      <c r="CG4" s="38" t="s">
-        <v>194</v>
-      </c>
-      <c r="CH4" s="38" t="s">
-        <v>195</v>
-      </c>
-      <c r="CI4" s="38" t="s">
-        <v>277</v>
-      </c>
       <c r="CJ4" s="38" t="s">
-        <v>196</v>
+        <v>280</v>
       </c>
       <c r="CK4" s="38" t="s">
-        <v>290</v>
+        <v>199</v>
       </c>
       <c r="CL4" s="38" t="s">
         <v>293</v>
       </c>
       <c r="CM4" s="38" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="CN4" s="38" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="CO4" s="38" t="s">
-        <v>185</v>
+        <v>300</v>
       </c>
       <c r="CP4" s="38" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="CQ4" s="38" t="s">
-        <v>281</v>
+        <v>189</v>
       </c>
       <c r="CR4" s="38" t="s">
-        <v>187</v>
+        <v>284</v>
       </c>
       <c r="CS4" s="38" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="CT4" s="38" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="CU4" s="38" t="s">
-        <v>282</v>
+        <v>193</v>
       </c>
       <c r="CV4" s="38" t="s">
-        <v>189</v>
+        <v>285</v>
       </c>
       <c r="CW4" s="38" t="s">
-        <v>301</v>
+        <v>192</v>
       </c>
       <c r="CX4" s="38" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="CY4" s="38" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="CZ4" s="38" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="DA4" s="38" t="s">
-        <v>161</v>
+        <v>310</v>
       </c>
       <c r="DB4" s="38" t="s">
-        <v>118</v>
+        <v>164</v>
       </c>
       <c r="DC4" s="38" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="DD4" s="38" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
       <c r="DE4" s="38" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="DF4" s="38" t="s">
-        <v>120</v>
+        <v>165</v>
       </c>
       <c r="DG4" s="38" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="DH4" s="38" t="s">
-        <v>164</v>
+        <v>124</v>
       </c>
       <c r="DI4" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="DJ4" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="DK4" s="38" t="s">
+        <v>241</v>
+      </c>
+      <c r="DL4" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="DM4" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="DN4" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="DO4" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="DP4" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="DQ4" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="DR4" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="DS4" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="DT4" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="DU4" s="38" t="s">
+        <v>246</v>
+      </c>
+      <c r="DV4" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="DW4" s="38" t="s">
+        <v>247</v>
+      </c>
+      <c r="DX4" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="DY4" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="DZ4" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="EA4" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="EB4" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="EC4" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="ED4" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="EE4" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="EF4" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="EG4" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="EH4" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="EI4" s="38" t="s">
+        <v>254</v>
+      </c>
+      <c r="EJ4" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="EK4" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="EL4" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="EM4" s="38" t="s">
+        <v>256</v>
+      </c>
+      <c r="EN4" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="EO4" s="41" t="s">
+        <v>257</v>
+      </c>
+      <c r="EP4" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="EQ4" s="38" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:147" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="58" t="s">
+        <v>205</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="L5" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" s="67" t="s">
+        <v>377</v>
+      </c>
+      <c r="O5" s="67" t="s">
+        <v>387</v>
+      </c>
+      <c r="P5" s="67" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q5" s="65" t="s">
+        <v>159</v>
+      </c>
+      <c r="R5" s="67" t="s">
+        <v>389</v>
+      </c>
+      <c r="S5" s="67" t="s">
+        <v>390</v>
+      </c>
+      <c r="T5" s="65" t="s">
+        <v>391</v>
+      </c>
+      <c r="U5" s="65" t="s">
+        <v>159</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="W5" s="53" t="s">
+        <v>330</v>
+      </c>
+      <c r="X5" s="53" t="s">
+        <v>331</v>
+      </c>
+      <c r="Y5" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="Z5" s="53" t="s">
+        <v>333</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="AC5" s="53" t="s">
+        <v>337</v>
+      </c>
+      <c r="AD5" s="53" t="s">
+        <v>340</v>
+      </c>
+      <c r="AE5" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="AF5" s="53" t="s">
+        <v>344</v>
+      </c>
+      <c r="AG5" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="AH5" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="AL5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="DJ4" s="38" t="s">
-        <v>238</v>
-      </c>
-      <c r="DK4" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="DL4" s="38" t="s">
-        <v>239</v>
-      </c>
-      <c r="DM4" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="DN4" s="38" t="s">
-        <v>240</v>
-      </c>
-      <c r="DO4" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="DP4" s="38" t="s">
-        <v>241</v>
-      </c>
-      <c r="DQ4" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="DR4" s="38" t="s">
-        <v>242</v>
-      </c>
-      <c r="DS4" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="DT4" s="38" t="s">
-        <v>243</v>
-      </c>
-      <c r="DU4" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="DV4" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="DW4" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="DX4" s="38" t="s">
-        <v>245</v>
-      </c>
-      <c r="DY4" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="DZ4" s="38" t="s">
-        <v>247</v>
-      </c>
-      <c r="EA4" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="EB4" s="38" t="s">
-        <v>248</v>
-      </c>
-      <c r="EC4" s="38" t="s">
+      <c r="AM5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN5" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="AO5" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="AP5" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="AQ5" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="AR5" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="AS5" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="AT5" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="AU5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AV5" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="AW5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AX5" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="AY5" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="AZ5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA5" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="BB5" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="BC5" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="BD5" s="53" t="s">
+        <v>366</v>
+      </c>
+      <c r="BE5" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="BF5" s="53" t="s">
+        <v>370</v>
+      </c>
+      <c r="BG5" s="53" t="s">
+        <v>372</v>
+      </c>
+      <c r="BH5" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="BI5" s="53" t="s">
+        <v>376</v>
+      </c>
+      <c r="BJ5" s="75" t="s">
+        <v>406</v>
+      </c>
+      <c r="BK5" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="ED4" s="38" t="s">
-        <v>249</v>
-      </c>
-      <c r="EE4" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="EF4" s="38" t="s">
-        <v>250</v>
-      </c>
-      <c r="EG4" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="EH4" s="38" t="s">
-        <v>251</v>
-      </c>
-      <c r="EI4" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="EJ4" s="38" t="s">
-        <v>252</v>
-      </c>
-      <c r="EK4" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="EL4" s="38" t="s">
-        <v>253</v>
-      </c>
-      <c r="EM4" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="EN4" s="40" t="s">
-        <v>254</v>
-      </c>
-      <c r="EO4" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="EP4" s="38" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="5" spans="1:146" ht="57.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="56" t="s">
-        <v>202</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="K5" s="45" t="s">
-        <v>157</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" s="65" t="s">
-        <v>374</v>
-      </c>
-      <c r="N5" s="65" t="s">
-        <v>384</v>
-      </c>
-      <c r="O5" s="65" t="s">
-        <v>385</v>
-      </c>
-      <c r="P5" s="63" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q5" s="65" t="s">
-        <v>386</v>
-      </c>
-      <c r="R5" s="65" t="s">
-        <v>387</v>
-      </c>
-      <c r="S5" s="63" t="s">
-        <v>388</v>
-      </c>
-      <c r="T5" s="63" t="s">
-        <v>156</v>
-      </c>
-      <c r="U5" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="V5" s="52" t="s">
-        <v>327</v>
-      </c>
-      <c r="W5" s="52" t="s">
-        <v>328</v>
-      </c>
-      <c r="X5" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="Y5" s="52" t="s">
-        <v>330</v>
-      </c>
-      <c r="Z5" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="AA5" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="AB5" s="52" t="s">
-        <v>334</v>
-      </c>
-      <c r="AC5" s="52" t="s">
-        <v>337</v>
-      </c>
-      <c r="AD5" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="AE5" s="52" t="s">
-        <v>341</v>
-      </c>
-      <c r="AF5" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="AG5" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AJ5" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="AK5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="AL5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AM5" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="AN5" s="6" t="s">
-        <v>349</v>
-      </c>
-      <c r="AO5" s="6" t="s">
-        <v>351</v>
-      </c>
-      <c r="AP5" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="AQ5" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="AR5" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="AS5" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="AT5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="AU5" s="52" t="s">
-        <v>94</v>
-      </c>
-      <c r="AV5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AW5" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="AX5" s="52" t="s">
-        <v>89</v>
-      </c>
-      <c r="AY5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AZ5" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="BA5" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="BB5" s="4" t="s">
-        <v>361</v>
-      </c>
-      <c r="BC5" s="52" t="s">
-        <v>363</v>
-      </c>
-      <c r="BD5" s="4" t="s">
-        <v>364</v>
-      </c>
-      <c r="BE5" s="52" t="s">
-        <v>367</v>
-      </c>
-      <c r="BF5" s="52" t="s">
-        <v>369</v>
-      </c>
-      <c r="BG5" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="BH5" s="52" t="s">
-        <v>373</v>
-      </c>
-      <c r="BI5" s="73" t="s">
-        <v>403</v>
-      </c>
-      <c r="BJ5" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="BK5" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="BL5" s="4" t="s">
         <v>43</v>
       </c>
       <c r="BM5" s="4" t="s">
-        <v>258</v>
+        <v>44</v>
       </c>
       <c r="BN5" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="BO5" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="BP5" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="BQ5" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="BR5" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="BS5" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="BT5" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="BU5" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="BV5" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="BO5" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="BP5" s="4" t="s">
+      <c r="BW5" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="BX5" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="BY5" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="BQ5" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="BR5" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="BS5" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="BT5" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="BU5" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="BV5" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="BW5" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="BX5" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="BY5" s="4" t="s">
-        <v>311</v>
-      </c>
       <c r="BZ5" s="4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="CA5" s="4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="CB5" s="4" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="CC5" s="4" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="CD5" s="4" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CE5" s="4" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CF5" s="4" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CG5" s="4" t="s">
-        <v>286</v>
+        <v>328</v>
       </c>
       <c r="CH5" s="4" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="CI5" s="4" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="CJ5" s="4" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="CK5" s="4" t="s">
         <v>292</v>
       </c>
       <c r="CL5" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="CM5" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="CN5" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="CO5" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="CM5" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="CN5" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="CO5" s="4" t="s">
-        <v>298</v>
-      </c>
       <c r="CP5" s="4" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="CQ5" s="4" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="CR5" s="4" t="s">
-        <v>279</v>
+        <v>303</v>
       </c>
       <c r="CS5" s="4" t="s">
-        <v>191</v>
+        <v>282</v>
       </c>
       <c r="CT5" s="4" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="CU5" s="4" t="s">
-        <v>283</v>
+        <v>195</v>
       </c>
       <c r="CV5" s="4" t="s">
-        <v>266</v>
+        <v>286</v>
       </c>
       <c r="CW5" s="4" t="s">
-        <v>302</v>
+        <v>269</v>
       </c>
       <c r="CX5" s="4" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="CY5" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="CZ5" s="4" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="DA5" s="4" t="s">
-        <v>166</v>
+        <v>311</v>
       </c>
       <c r="DB5" s="4" t="s">
-        <v>122</v>
+        <v>169</v>
       </c>
       <c r="DC5" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="DD5" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="DE5" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="DF5" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="DG5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="DH5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="DI5" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="DE5" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="DF5" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="DG5" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="DH5" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="DI5" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="DJ5" s="4" t="s">
-        <v>237</v>
+        <v>39</v>
       </c>
       <c r="DK5" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="DL5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="DM5" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="DN5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="DO5" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="DP5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="DQ5" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="DR5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="DL5" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="DM5" s="7" t="s">
+      <c r="DS5" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="DT5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="DN5" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="DO5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="DP5" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="DQ5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="DR5" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="DS5" s="7" t="s">
+      <c r="DU5" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="DV5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="DW5" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="DX5" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="DY5" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="DZ5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="DT5" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="DU5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="DV5" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="DW5" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="DX5" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="DY5" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="DZ5" s="4" t="s">
-        <v>221</v>
-      </c>
       <c r="EA5" s="4" t="s">
-        <v>143</v>
+        <v>224</v>
       </c>
       <c r="EB5" s="4" t="s">
-        <v>219</v>
+        <v>146</v>
       </c>
       <c r="EC5" s="4" t="s">
-        <v>114</v>
+        <v>222</v>
       </c>
       <c r="ED5" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="EE5" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="EF5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="EE5" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="EF5" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="EG5" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="EH5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="EI5" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="EG5" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="EH5" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="EI5" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="EJ5" s="4" t="s">
-        <v>211</v>
+      <c r="EJ5" s="7" t="s">
+        <v>152</v>
       </c>
       <c r="EK5" s="4" t="s">
-        <v>151</v>
+        <v>214</v>
       </c>
       <c r="EL5" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="EM5" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="EN5" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="EO5" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="EM5" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="EN5" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="EO5" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="EP5" s="4" t="s">
-        <v>205</v>
+      <c r="EP5" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="EQ5" s="4" t="s">
+        <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:146" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="M6" s="62"/>
-      <c r="N6" s="62"/>
-      <c r="O6" s="62"/>
-      <c r="Q6" s="62"/>
-      <c r="R6" s="62"/>
-      <c r="S6" s="62"/>
+    <row r="6" spans="1:147" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="N6" s="64"/>
+      <c r="O6" s="64"/>
+      <c r="P6" s="64"/>
+      <c r="R6" s="64"/>
+      <c r="S6" s="64"/>
+      <c r="T6" s="64"/>
     </row>
-    <row r="7" spans="1:146" x14ac:dyDescent="0.25">
-      <c r="G7" s="32"/>
-      <c r="M7" s="62"/>
-      <c r="N7" s="62"/>
-      <c r="O7" s="62"/>
-      <c r="Q7" s="62"/>
-      <c r="R7" s="62"/>
-      <c r="S7" s="62"/>
+    <row r="7" spans="1:147" x14ac:dyDescent="0.55000000000000004">
+      <c r="H7" s="32"/>
+      <c r="N7" s="64"/>
+      <c r="O7" s="64"/>
+      <c r="P7" s="64"/>
+      <c r="R7" s="64"/>
+      <c r="S7" s="64"/>
+      <c r="T7" s="64"/>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I6:I1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Class,Collection,File,Fonds,Item,Other Level,Record Group,Series,Sub-Fonds,Sub-Group,Sub-Series"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6:K1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L6:L1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X6:X1048576 AD6:AD1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y6:Y1048576 AE6:AE1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"bulk,single,inclusive"</formula1>
     </dataValidation>
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="G6:G1048576" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="H6:H1048576" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>1</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J6:J1048576 EN6:EN1048576 EL6:EL1048576 EP6:EP1048576 EJ6:EJ1048576 EH6:EH1048576 EF6:EF1048576 ED6:ED1048576 EB6:EB1048576 DZ6:DZ1048576 DX6:DX1048576 DV6:DV1048576 DT6:DT1048576 DR6:DR1048576 DP6:DP1048576 DN6:DN1048576 DL6:DL1048576 DJ6:DJ1048576 P6:P1048576 T6:T1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="K6:K1048576 EO6:EO1048576 EM6:EM1048576 EQ6:EQ1048576 EK6:EK1048576 EI6:EI1048576 EG6:EG1048576 EE6:EE1048576 EC6:EC1048576 EA6:EA1048576 DY6:DY1048576 DW6:DW1048576 DU6:DU1048576 DS6:DS1048576 DQ6:DQ1048576 DO6:DO1048576 DM6:DM1048576 DK6:DK1048576 Q6:Q1048576 U6:U1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4116,7 +4157,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>BO6:BO1048576 BS6:BS1048576 CI6:CI1048576 BW6:BW1048576 CU6:CU1048576 CM6:CM1048576 CQ6:CQ1048576 CY6:CY1048576 CA6:CA1048576 CE6:CE1048576</xm:sqref>
+          <xm:sqref>BP6:BP1048576 BT6:BT1048576 CJ6:CJ1048576 BX6:BX1048576 CV6:CV1048576 CN6:CN1048576 CR6:CR1048576 CZ6:CZ1048576 CB6:CB1048576 CF6:CF1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4132,50 +4173,50 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="128.28515625" customWidth="1"/>
-    <col min="2" max="1025" width="8.42578125"/>
+    <col min="1" max="1" width="128.26171875" customWidth="1"/>
+    <col min="2" max="1025" width="8.578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="17" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="47" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -4192,24 +4233,24 @@
       <selection activeCell="D9" sqref="D9:D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>